<commit_message>
remove timezone fixes (stick with Toronto timezone)
</commit_message>
<xml_diff>
--- a/data/FIXED_Pool_data_May_2024_CAPITALIZATION.xlsx
+++ b/data/FIXED_Pool_data_May_2024_CAPITALIZATION.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Jan 01 2021" sheetId="1" state="visible" r:id="rId2"/>
@@ -315,10 +315,10 @@
     <t xml:space="preserve">Charleston, South Carolina, United States</t>
   </si>
   <si>
-    <t xml:space="preserve">ULTIMUS</t>
+    <t xml:space="preserve">ULTIMUSPOOL</t>
   </si>
   <si>
-    <t xml:space="preserve">SecPool</t>
+    <t xml:space="preserve">SECPOOL</t>
   </si>
 </sst>
 </file>
@@ -772,9 +772,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1204920</xdr:colOff>
+      <xdr:colOff>1204560</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>144360</xdr:rowOff>
+      <xdr:rowOff>144000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -784,7 +784,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="901800" y="3537000"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -812,9 +812,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -824,7 +824,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="2979360"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -852,9 +852,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>112680</xdr:rowOff>
+      <xdr:rowOff>112320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -864,7 +864,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="3505320"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -892,9 +892,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1141200</xdr:colOff>
+      <xdr:colOff>1140840</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>64800</xdr:rowOff>
+      <xdr:rowOff>64440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -904,7 +904,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="838080" y="5257800"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -932,9 +932,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1243080</xdr:colOff>
+      <xdr:colOff>1242720</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>58680</xdr:rowOff>
+      <xdr:rowOff>58320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -944,7 +944,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="939960" y="5251680"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -972,9 +972,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -984,7 +984,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="5505480"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1012,9 +1012,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
+      <xdr:rowOff>5760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1024,7 +1024,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="920520"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1052,9 +1052,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1064,7 +1064,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="876240"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1092,9 +1092,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1104,7 +1104,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="700920"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1132,9 +1132,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1144,7 +1144,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="1051560"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1172,9 +1172,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1230120</xdr:colOff>
+      <xdr:colOff>1229760</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>58680</xdr:rowOff>
+      <xdr:rowOff>58320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1184,7 +1184,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="927000" y="8452080"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1212,9 +1212,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1224,7 +1224,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="8705880"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1252,9 +1252,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1211040</xdr:colOff>
+      <xdr:colOff>1210680</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>101520</xdr:rowOff>
+      <xdr:rowOff>101160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1264,7 +1264,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="907920" y="2418120"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1292,9 +1292,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1304,7 +1304,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="1927800"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1332,9 +1332,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>137520</xdr:rowOff>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1344,7 +1344,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="2629080"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1372,9 +1372,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1384,7 +1384,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="1752480"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1412,9 +1412,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1424,7 +1424,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="175320"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1452,9 +1452,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1464,7 +1464,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="175320"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1492,9 +1492,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1504,7 +1504,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="2804040"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1532,9 +1532,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>112680</xdr:rowOff>
+      <xdr:rowOff>112320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1544,7 +1544,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="4105440"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1572,9 +1572,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1584,7 +1584,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="4305240"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1612,9 +1612,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1624,7 +1624,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="6505560"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1652,9 +1652,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1664,7 +1664,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="6305400"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1692,9 +1692,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1704,7 +1704,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="7905600"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1732,9 +1732,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>112680</xdr:rowOff>
+      <xdr:rowOff>112320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1744,7 +1744,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="7305840"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1772,9 +1772,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>112680</xdr:rowOff>
+      <xdr:rowOff>112320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1784,7 +1784,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="6105600"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1812,9 +1812,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1824,7 +1824,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="7105680"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1852,9 +1852,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1864,7 +1864,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="7505640"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1892,9 +1892,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1904,7 +1904,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="6905520"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1932,9 +1932,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1944,7 +1944,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="4905360"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1972,9 +1972,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1984,7 +1984,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="4905360"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2012,9 +2012,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>112680</xdr:rowOff>
+      <xdr:rowOff>112320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2024,7 +2024,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="8906040"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2052,9 +2052,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2064,7 +2064,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="8105760"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2092,9 +2092,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1204920</xdr:colOff>
+      <xdr:colOff>1204560</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>144000</xdr:rowOff>
+      <xdr:rowOff>143640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2104,7 +2104,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="901800" y="5337000"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2132,9 +2132,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1204920</xdr:colOff>
+      <xdr:colOff>1204560</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>144360</xdr:rowOff>
+      <xdr:rowOff>144000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2144,7 +2144,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="901800" y="5137200"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2172,9 +2172,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1179360</xdr:colOff>
+      <xdr:colOff>1179000</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>96840</xdr:rowOff>
+      <xdr:rowOff>96480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2184,7 +2184,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="876240" y="5689800"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2212,9 +2212,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1179360</xdr:colOff>
+      <xdr:colOff>1179000</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>146520</xdr:rowOff>
+      <xdr:rowOff>146160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2224,7 +2224,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="876240" y="710280"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2252,9 +2252,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1179360</xdr:colOff>
+      <xdr:colOff>1179000</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>146520</xdr:rowOff>
+      <xdr:rowOff>146160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2264,7 +2264,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="876240" y="534960"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2292,9 +2292,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1179360</xdr:colOff>
+      <xdr:colOff>1179000</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>146160</xdr:rowOff>
+      <xdr:rowOff>145800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2304,7 +2304,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="876240" y="1060560"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2332,9 +2332,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1179360</xdr:colOff>
+      <xdr:colOff>1179000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>146160</xdr:rowOff>
+      <xdr:rowOff>145800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2344,7 +2344,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="876240" y="885240"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2377,9 +2377,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1204920</xdr:colOff>
+      <xdr:colOff>1204560</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>144360</xdr:rowOff>
+      <xdr:rowOff>144000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2389,7 +2389,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="901800" y="3537000"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2417,9 +2417,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2429,7 +2429,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="2979360"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2457,9 +2457,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>112680</xdr:rowOff>
+      <xdr:rowOff>112320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2469,7 +2469,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="3505320"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2497,9 +2497,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1141200</xdr:colOff>
+      <xdr:colOff>1140840</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>64800</xdr:rowOff>
+      <xdr:rowOff>64440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2509,7 +2509,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="838080" y="5257800"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2537,9 +2537,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1243080</xdr:colOff>
+      <xdr:colOff>1242720</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>58680</xdr:rowOff>
+      <xdr:rowOff>58320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2549,7 +2549,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="939960" y="5251680"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2577,9 +2577,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2589,7 +2589,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="5505480"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2617,9 +2617,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
+      <xdr:rowOff>5760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2629,7 +2629,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="920520"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2657,9 +2657,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2669,7 +2669,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="876240"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2697,9 +2697,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2709,7 +2709,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="700920"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2737,9 +2737,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2749,7 +2749,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="1051560"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2777,9 +2777,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1230120</xdr:colOff>
+      <xdr:colOff>1229760</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>58680</xdr:rowOff>
+      <xdr:rowOff>58320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2789,7 +2789,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="927000" y="8452080"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2817,9 +2817,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2829,7 +2829,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="8705880"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2857,9 +2857,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1211040</xdr:colOff>
+      <xdr:colOff>1210680</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>101520</xdr:rowOff>
+      <xdr:rowOff>101160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2869,7 +2869,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="907920" y="2418120"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2897,9 +2897,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2909,7 +2909,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="1927800"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2937,9 +2937,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>137520</xdr:rowOff>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2949,7 +2949,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="2629080"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2977,9 +2977,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2989,7 +2989,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="1752480"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3017,9 +3017,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3029,7 +3029,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="175320"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3057,9 +3057,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3069,7 +3069,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="175320"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3097,9 +3097,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3109,7 +3109,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="2804040"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3137,9 +3137,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>112680</xdr:rowOff>
+      <xdr:rowOff>112320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3149,7 +3149,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="4105440"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3177,9 +3177,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3189,7 +3189,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="4305240"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3217,9 +3217,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3229,7 +3229,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="6505560"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3257,9 +3257,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3269,7 +3269,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="6305400"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3297,9 +3297,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3309,7 +3309,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="7905600"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3337,9 +3337,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>112680</xdr:rowOff>
+      <xdr:rowOff>112320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3349,7 +3349,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="7305840"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3377,9 +3377,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>112680</xdr:rowOff>
+      <xdr:rowOff>112320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3389,7 +3389,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="6105600"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3417,9 +3417,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3429,7 +3429,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="7105680"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3457,9 +3457,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3469,7 +3469,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="7505640"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3497,9 +3497,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3509,7 +3509,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="6905520"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3537,9 +3537,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3549,7 +3549,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="4905360"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3577,9 +3577,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3589,7 +3589,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="4905360"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3617,9 +3617,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>112680</xdr:rowOff>
+      <xdr:rowOff>112320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3629,7 +3629,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="8906040"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3657,9 +3657,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3669,7 +3669,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2690640" y="8105760"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3697,9 +3697,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1204920</xdr:colOff>
+      <xdr:colOff>1204560</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>144000</xdr:rowOff>
+      <xdr:rowOff>143640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3709,7 +3709,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="901800" y="5337000"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3737,9 +3737,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1204920</xdr:colOff>
+      <xdr:colOff>1204560</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>144360</xdr:rowOff>
+      <xdr:rowOff>144000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3749,7 +3749,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="901800" y="5137200"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3777,9 +3777,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1179360</xdr:colOff>
+      <xdr:colOff>1179000</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>96840</xdr:rowOff>
+      <xdr:rowOff>96480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3789,7 +3789,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="876240" y="5689800"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3817,9 +3817,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1179360</xdr:colOff>
+      <xdr:colOff>1179000</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>146520</xdr:rowOff>
+      <xdr:rowOff>146160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3829,7 +3829,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="876240" y="710280"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3857,9 +3857,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1179360</xdr:colOff>
+      <xdr:colOff>1179000</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>146520</xdr:rowOff>
+      <xdr:rowOff>146160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3869,7 +3869,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="876240" y="534960"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3897,9 +3897,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1179360</xdr:colOff>
+      <xdr:colOff>1179000</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>146160</xdr:rowOff>
+      <xdr:rowOff>145800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3909,7 +3909,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="876240" y="1060560"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3937,9 +3937,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1179360</xdr:colOff>
+      <xdr:colOff>1179000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>146160</xdr:rowOff>
+      <xdr:rowOff>145800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3949,7 +3949,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="876240" y="885240"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3982,9 +3982,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3994,7 +3994,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1693440" y="9105840"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4022,9 +4022,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4034,7 +4034,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1693440" y="9105840"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4067,9 +4067,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4079,7 +4079,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1187280" y="6004440"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4107,9 +4107,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4119,7 +4119,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1187280" y="6004440"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4152,9 +4152,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>112680</xdr:rowOff>
+      <xdr:rowOff>112320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4164,7 +4164,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1187280" y="4505400"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4192,9 +4192,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>112680</xdr:rowOff>
+      <xdr:rowOff>112320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4204,7 +4204,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1187280" y="4505400"/>
-          <a:ext cx="303120" cy="312480"/>
+          <a:ext cx="302760" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4237,9 +4237,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>750960</xdr:colOff>
+      <xdr:colOff>750600</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>101880</xdr:rowOff>
+      <xdr:rowOff>101520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4249,7 +4249,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="563400" y="3995640"/>
-          <a:ext cx="187560" cy="312480"/>
+          <a:ext cx="187200" cy="312120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4317,7 +4317,7 @@
   </sheetPr>
   <dimension ref="A1:F998"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
     </sheetView>
   </sheetViews>
@@ -8287,7 +8287,7 @@
       <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="33.48"/>
@@ -10270,7 +10270,7 @@
       <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="16.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="40.83"/>
@@ -11933,10 +11933,10 @@
   <dimension ref="A1:F985"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="topLeft" activeCell="P13" activeCellId="0" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="16.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="40.83"/>
@@ -13467,11 +13467,11 @@
   </sheetPr>
   <dimension ref="A1:F925"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="31.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="43"/>
@@ -15540,10 +15540,10 @@
   </sheetPr>
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
+      <selection pane="bottomLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>